<commit_message>
2do obj con días, funciones out calendario específico
</commit_message>
<xml_diff>
--- a/Interrogaciones/src/instancia_datos/listado_cursos.xlsx
+++ b/Interrogaciones/src/instancia_datos/listado_cursos.xlsx
@@ -443,273 +443,273 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>IEE2463-1</t>
+          <t>ICS2523-3</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ICE3613-1</t>
+          <t>IEE2463-1</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ICE3124-1</t>
+          <t>ICE2533-1</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ICH2214-1</t>
+          <t>ICE3753-1</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>IMT3150-1</t>
+          <t>IIC2764-1</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ICC2105-1</t>
+          <t>ICE3653-1</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>ICS2563-1</t>
+          <t>IMM2053-1</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>ICC3543-1</t>
+          <t>IIC2333-1</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>IIQ2673-1</t>
+          <t>ICC2514-1</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>IEE2213-1</t>
+          <t>IIQ2133-1</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ICS3413-1</t>
+          <t>ICM2022-1</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>IIC2733-1</t>
+          <t>IIC3143-1</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ICE2604-1</t>
+          <t>ICC3214-1</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>IEE3234-1</t>
+          <t>ICS3413-1</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>ICH3364-1</t>
+          <t>ICE3124-1</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ICM2803-1</t>
+          <t>ICE3613-1</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>IIC2733-2</t>
+          <t>IEE2213-1</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>IIQ3343-1</t>
+          <t>IMT3150-1</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>IEE2123-1</t>
+          <t>IIQ3343-1</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>IMM2053-1</t>
+          <t>ICE2604-1</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>ICE3653-1</t>
+          <t>IIQ2673-1</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>ICS2523-3</t>
+          <t>IIC2733-1</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>ICE2533-1</t>
+          <t>ICC2105-1</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>IIC2764-1</t>
+          <t>IEE3234-1</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>ICE3753-1</t>
+          <t>ICC3543-1</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>IMM2033-1</t>
+          <t>ICH3364-1</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>ICH1005-1</t>
+          <t>IEE2123-1</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>ICH3350-1</t>
+          <t>ICH2214-1</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>IMT3800-1</t>
+          <t>IIC2733-2</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>IMM2003-1</t>
+          <t>ICS2563-1</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>ICS3582-1</t>
+          <t>ICM2803-1</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>ICE2028-1</t>
+          <t>ICH1005-1</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>ICM3762-1</t>
+          <t>IMM2033-1</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>IIC3800-1</t>
+          <t>ICH3350-1</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>ICS2121-1</t>
+          <t>ICM1001-1</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>IMM3800-1</t>
+          <t>IIC1001-1</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>IMM2013-1</t>
+          <t>ICH3222-1</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>ICM1001-1</t>
+          <t>ICC3124-1</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>ICC3124-1</t>
+          <t>ICM2223-1</t>
         </is>
       </c>
     </row>
@@ -723,14 +723,14 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>IIC1001-1</t>
+          <t>IIQ2003-1</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>ICM2223-1</t>
+          <t>ICE3233-1</t>
         </is>
       </c>
     </row>
@@ -744,679 +744,679 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>ICE3233-1</t>
+          <t>IMM2013-1</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>IIQ2003-1</t>
+          <t>ICS2123-3</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>ICH3222-1</t>
+          <t>IIC2613-1</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>IEE3732-1</t>
+          <t>ICE2006-1</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>ICT3623-1</t>
+          <t>IMM2213-1</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>IIC2213-1</t>
+          <t>ICE2114-1</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>IIC3103-1</t>
+          <t>ICM2313-1</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>ICE2006-1</t>
+          <t>ICT3523-1</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>ICM3251-1</t>
+          <t>IIC3113-1</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>IEE3373-1</t>
+          <t>IEE2343-1</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>ICE2114-1</t>
+          <t>IIC3113-2</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>IMT2111-1</t>
+          <t>ICT2303-1</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>ICS3762-1</t>
+          <t>IEE2513-1</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>IIQ3643-1</t>
+          <t>ICC3253-1</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>ICC3264-1</t>
+          <t>ICM2203-1</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>ICH2124-1</t>
+          <t>ICH2574-1</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>IEE2103-1</t>
+          <t>ICE2020-1</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>ICE2313-1</t>
+          <t>IMM2003-1</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>IEE2613-1</t>
+          <t>IMM3313-1</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>IEE2413-1</t>
+          <t>ICH3532-1</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>IMM3313-1</t>
+          <t>ICE2028-1</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>ICH2114-1</t>
+          <t>ICH3374-1</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>IIC3757-1</t>
+          <t>ICH2304-1</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>IMM2043-1</t>
+          <t>ICH2204-1</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>ICH3532-1</t>
+          <t>ICC3434-1</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>ICE2020-1</t>
+          <t>IEE2113-1</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>ICH2574-1</t>
+          <t>ICM2333-1</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>ICC3434-1</t>
+          <t>ICM3235-1</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>ICH2204-1</t>
+          <t>ICS3313-1</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>IEE2113-1</t>
+          <t>ICM2213-1</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>ICH3374-1</t>
+          <t>IMM2043-1</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>ICH2304-1</t>
+          <t>ICS3811-1</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>IIC2713-1</t>
+          <t>ICC2204-1</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>IIC2713-3</t>
+          <t>ICE2633-1</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>ICM3243-1</t>
+          <t>ICS3723-1</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>ICS2023-1</t>
+          <t>IIQ2303-1</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>ICT3464-1</t>
+          <t>ICE2703-1</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>IIC2713-2</t>
+          <t>ICT3283-1</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>ICC2304-1</t>
+          <t>ICS2123-1</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>ICH2304-2</t>
+          <t>ICE3443-1</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>IEE2713-1</t>
+          <t>ICS3151-1</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>ICH3600-1</t>
+          <t>IMM3323-1</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>ICS2123-2</t>
+          <t>IIC3743-1</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>ICE2623-1</t>
+          <t>IIQ2043-1</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>IMM3323-1</t>
+          <t>IIC2133-1</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>ICS3811-1</t>
+          <t>IIC2133-2</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>IIC3743-1</t>
+          <t>ICE3663-1</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>ICE2703-1</t>
+          <t>ICH2114-1</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>IIQ2303-1</t>
+          <t>ICM2403-1</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>ICC2204-1</t>
+          <t>ICE3513-1</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>ICE3443-1</t>
+          <t>IIC3242-1</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>ICM3235-1</t>
+          <t>ICC1001-1</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>ICM2213-1</t>
+          <t>IIC3757-1</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>ICS3151-1</t>
+          <t>ICE2623-1</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>ICS2123-1</t>
+          <t>IEE3732-1</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>ICM2333-1</t>
+          <t>IIC2213-1</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>ICS3723-1</t>
+          <t>ICT3623-1</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>ICS3313-1</t>
+          <t>IMM3800-1</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>ICE2633-1</t>
+          <t>ICH2304-2</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>ICT3283-1</t>
+          <t>ICS2123-2</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>ICM2413-1</t>
+          <t>IEE2713-1</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>IIC2143-1</t>
+          <t>IIC2713-1</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>ICT2233-1</t>
+          <t>ICH3600-1</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>ICS2563-2</t>
+          <t>ICS2023-1</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>IMT3130-1</t>
+          <t>ICM3243-1</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>ICM2003-1</t>
+          <t>ICT3464-1</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>ICM2028-1</t>
+          <t>ICC2304-1</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>IIC2143-2</t>
+          <t>IIC2713-3</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>ICT3435-1</t>
+          <t>IIC2713-2</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>IIQ2663-1</t>
+          <t>ICM3762-1</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>ICE3413-1</t>
+          <t>ICS2121-1</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>IEE2513-1</t>
+          <t>ICS3582-1</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>ICM2313-1</t>
+          <t>IMT3800-1</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>ICM2203-1</t>
+          <t>IEE2413-1</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>ICT2303-1</t>
+          <t>IIQ2663-1</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>IIC3113-1</t>
+          <t>ICH2124-1</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>ICC3253-1</t>
+          <t>ICT2233-1</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>IMM2213-1</t>
+          <t>ICS2563-2</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>IIC2613-1</t>
+          <t>ICE3413-1</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>IIC3113-2</t>
+          <t>ICM2003-1</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>IEE2343-1</t>
+          <t>IEE2103-1</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>ICT3523-1</t>
+          <t>IIC2143-2</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>ICS2123-3</t>
+          <t>IIC2143-1</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>IIC2133-1</t>
+          <t>ICM2413-1</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>ICC1001-1</t>
+          <t>ICE2313-1</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>ICM2403-1</t>
+          <t>IEE2613-1</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>ICE3513-1</t>
+          <t>ICT3435-1</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>ICE3663-1</t>
+          <t>IMT3130-1</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>IIQ2043-1</t>
+          <t>ICM2028-1</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>IIC2133-2</t>
+          <t>IEE3373-1</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>IIC3242-1</t>
+          <t>IMT2111-1</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>IIQ2133-1</t>
+          <t>ICM3251-1</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>ICC3214-1</t>
+          <t>IIC3800-1</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>IIC3143-1</t>
+          <t>ICS3762-1</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>IIC2333-1</t>
+          <t>IIQ3643-1</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>ICM2022-1</t>
+          <t>ICC3264-1</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>ICC2514-1</t>
+          <t>IIC3103-1</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Inclusión cursos FIS, QIM. I2 en obj2 y Restr 2 dias consecutivos sin prueba
</commit_message>
<xml_diff>
--- a/Interrogaciones/src/instancia_datos/listado_cursos.xlsx
+++ b/Interrogaciones/src/instancia_datos/listado_cursos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A173"/>
+  <dimension ref="A1:A177"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,917 +443,917 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ICS2523-3</t>
+          <t>IMM2043-1</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>IEE2463-1</t>
+          <t>ICC2204-1</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ICE2533-1</t>
+          <t>ICH2204-1</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ICE3753-1</t>
+          <t>IMM3323-1</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>IIC2764-1</t>
+          <t>ICH3374-1</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ICE3653-1</t>
+          <t>ICM2213-1</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>IMM2053-1</t>
+          <t>ICE2633-1</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>IIC2333-1</t>
+          <t>ICM2333-1</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>ICC2514-1</t>
+          <t>ICE2703-1</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>IIQ2133-1</t>
+          <t>IMM2013-1</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ICM2022-1</t>
+          <t>ICS3151-1</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>IIC3143-1</t>
+          <t>ICS3313-1</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ICC3214-1</t>
+          <t>ICT3283-1</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ICS3413-1</t>
+          <t>ICS3723-1</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>ICE3124-1</t>
+          <t>ICE3443-1</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ICE3613-1</t>
+          <t>ICH2304-1</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>IEE2213-1</t>
+          <t>ICE2020-1</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>IMT3150-1</t>
+          <t>IEE2113-1</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>IIQ3343-1</t>
+          <t>IIQ2303-1</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>ICE2604-1</t>
+          <t>ICM3235-1</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>IIQ2673-1</t>
+          <t>ICS2123-1</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>IIC2733-1</t>
+          <t>IMM3313-1</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>ICC2105-1</t>
+          <t>ICH2304-2</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>IEE3234-1</t>
+          <t>ICH1005-1</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>ICC3543-1</t>
+          <t>IEE2713-1</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>ICH3364-1</t>
+          <t>IIC2713-2</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>IEE2123-1</t>
+          <t>IIC2713-1</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>ICH2214-1</t>
+          <t>ICS2123-2</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>IIC2733-2</t>
+          <t>ICH3600-1</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>ICS2563-1</t>
+          <t>IIC2713-3</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>ICM2803-1</t>
+          <t>ICM3243-1</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>ICH1005-1</t>
+          <t>ICE2623-1</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>IMM2033-1</t>
+          <t>ICT3464-1</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>ICH3350-1</t>
+          <t>ICS2023-1</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>ICM1001-1</t>
+          <t>ICC2304-1</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>IIC1001-1</t>
+          <t>IEE3234-1</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>ICH3222-1</t>
+          <t>IEE2463-1</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>ICC3124-1</t>
+          <t>IIC2733-1</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>ICM2223-1</t>
+          <t>IMT3150-1</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>ICS2523-4</t>
+          <t>ICS3413-1</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>IIQ2003-1</t>
+          <t>IIQ3343-1</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>ICE3233-1</t>
+          <t>IEE2123-1</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>IMM1003-1</t>
+          <t>ICC3543-1</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>IMM2013-1</t>
+          <t>ICH3364-1</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>ICS2123-3</t>
+          <t>IIC2733-2</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>IIC2613-1</t>
+          <t>ICM2803-1</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>ICE2006-1</t>
+          <t>ICH2214-1</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>IMM2213-1</t>
+          <t>ICE3613-1</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>ICE2114-1</t>
+          <t>ICE2604-1</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>ICM2313-1</t>
+          <t>IEE2213-1</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>ICT3523-1</t>
+          <t>ICS2563-1</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>IIC3113-1</t>
+          <t>ICE3124-1</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>IEE2343-1</t>
+          <t>IIQ2673-1</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>IIC3113-2</t>
+          <t>ICC2105-1</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>ICT2303-1</t>
+          <t>ICH2574-1</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>IEE2513-1</t>
+          <t>ICH3532-1</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>ICC3253-1</t>
+          <t>ICC3434-1</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>ICM2203-1</t>
+          <t>ICE2028-1</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>ICH2574-1</t>
+          <t>IMM2003-1</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>ICE2020-1</t>
+          <t>ICE3653-1</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>IMM2003-1</t>
+          <t>ICS3811-1</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>IMM3313-1</t>
+          <t>IMM2033-1</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>ICH3532-1</t>
+          <t>IIC3103-1</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>ICE2028-1</t>
+          <t>ICH3350-1</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>ICH3374-1</t>
+          <t>IIC2764-1</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>ICH2304-1</t>
+          <t>ICE2313-1</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>ICH2204-1</t>
+          <t>IEE2103-1</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>ICC3434-1</t>
+          <t>IEE2613-1</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>IEE2113-1</t>
+          <t>IEE2413-1</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>ICM2333-1</t>
+          <t>ICH2124-1</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>ICM3235-1</t>
+          <t>IIQ3643-1</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>ICS3313-1</t>
+          <t>ICE2006-1</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>ICM2213-1</t>
+          <t>IMT2111-1</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>IMM2043-1</t>
+          <t>ICC3264-1</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>ICS3811-1</t>
+          <t>IEE3373-1</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>ICC2204-1</t>
+          <t>ICM3251-1</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>ICE2633-1</t>
+          <t>ICS3762-1</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>ICS3723-1</t>
+          <t>ICE2114-1</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>IIQ2303-1</t>
+          <t>ICS2123-3</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>ICE2703-1</t>
+          <t>IMM2213-1</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>ICT3283-1</t>
+          <t>IIC3113-2</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>ICS2123-1</t>
+          <t>IEE2513-1</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>ICE3443-1</t>
+          <t>ICM2313-1</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>ICS3151-1</t>
+          <t>ICC3253-1</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>IMM3323-1</t>
+          <t>IEE2343-1</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>IIC3743-1</t>
+          <t>ICM2203-1</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>IIQ2043-1</t>
+          <t>ICT2303-1</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>IIC2133-1</t>
+          <t>ICT3523-1</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>IIC2133-2</t>
+          <t>IIC2613-1</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>ICE3663-1</t>
+          <t>IIC3113-1</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>ICH2114-1</t>
+          <t>IIC3743-1</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>ICM2403-1</t>
+          <t>IMM2053-1</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>ICE3513-1</t>
+          <t>ICE2533-1</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>IIC3242-1</t>
+          <t>ICE3753-1</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>ICC1001-1</t>
+          <t>ICS2523-3</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>IIC3757-1</t>
+          <t>IMM1003-1</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>ICE2623-1</t>
+          <t>ICM2223-1</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>IEE3732-1</t>
+          <t>ICS2523-4</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>IIC2213-1</t>
+          <t>ICM1001-1</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>ICT3623-1</t>
+          <t>IIC1001-1</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>IMM3800-1</t>
+          <t>IIQ2003-1</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>ICH2304-2</t>
+          <t>ICC3124-1</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>ICS2123-2</t>
+          <t>ICE3233-1</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>IEE2713-1</t>
+          <t>ICH3222-1</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>IIC2713-1</t>
+          <t>IEE3732-1</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>ICH3600-1</t>
+          <t>IMT3800-1</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>ICS2023-1</t>
+          <t>ICM3762-1</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>ICM3243-1</t>
+          <t>ICS2121-1</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>ICT3464-1</t>
+          <t>IIC2213-1</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>ICC2304-1</t>
+          <t>ICS3582-1</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>IIC2713-3</t>
+          <t>ICT3623-1</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>IIC2713-2</t>
+          <t>IIC3800-1</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>ICM3762-1</t>
+          <t>IIC3757-1</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>ICS2121-1</t>
+          <t>IMM3800-1</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>ICS3582-1</t>
+          <t>IIQ2043-1</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>IMT3800-1</t>
+          <t>IIC2133-1</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>IEE2413-1</t>
+          <t>IIC3242-1</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>IIQ2663-1</t>
+          <t>IIC2133-2</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>ICH2124-1</t>
+          <t>ICE3513-1</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>ICT2233-1</t>
+          <t>ICH2114-1</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>ICS2563-2</t>
+          <t>ICE3663-1</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>ICE3413-1</t>
+          <t>ICM2403-1</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>ICM2003-1</t>
+          <t>ICC1001-1</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>IEE2103-1</t>
+          <t>ICT3435-1</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>IIC2143-2</t>
+          <t>IIC2143-1</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>IIC2143-1</t>
+          <t>IMT3130-1</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>ICM2413-1</t>
+          <t>ICT2233-1</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>ICE2313-1</t>
+          <t>ICM2003-1</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>IEE2613-1</t>
+          <t>ICM2413-1</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>ICT3435-1</t>
+          <t>IIC2143-2</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>IMT3130-1</t>
+          <t>IIQ2663-1</t>
         </is>
       </c>
     </row>
@@ -1367,56 +1367,56 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>IEE3373-1</t>
+          <t>ICS2563-2</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>IMT2111-1</t>
+          <t>ICE3413-1</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>ICM3251-1</t>
+          <t>IIC2333-1</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>IIC3800-1</t>
+          <t>ICC3214-1</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>ICS3762-1</t>
+          <t>ICC2514-1</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>IIQ3643-1</t>
+          <t>IIQ2133-1</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>ICC3264-1</t>
+          <t>IIC3143-1</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>IIC3103-1</t>
+          <t>ICM2022-1</t>
         </is>
       </c>
     </row>
@@ -1458,187 +1458,215 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>I5_MS1 - Macroseccion 1</t>
+          <t>FIS1514_Coordinado - Macroseccion</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>I6_MS1 - Macroseccion 1</t>
+          <t>FIS1523_Coordinado - Macroseccion</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>ICE1514_Coordinado - Macroseccion</t>
+          <t>FIS1533_Coordinado - Macroseccion</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>ICH1104_Coordinado - Macroseccion</t>
+          <t>I5_MS1 - Macroseccion 1</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>ICM2503_Coordinado - Macroseccion</t>
+          <t>I6_MS1 - Macroseccion 1</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>ICS1113_Coordinado - Macroseccion</t>
+          <t>ICE1514_Coordinado - Macroseccion</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>ICS1513_Coordinado - Macroseccion</t>
+          <t>ICH1104_Coordinado - Macroseccion</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>ICS2523_1_2_Sec_Coordinadas - Macroseccion</t>
+          <t>ICM2503_Coordinado - Macroseccion</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>ICS2613_Coordinado - Macroseccion</t>
+          <t>ICS1113_Coordinado - Macroseccion</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>ICS3213_Coordinado - Macroseccion</t>
+          <t>ICS1513_Coordinado - Macroseccion</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>ICS3313_2_3_Sec_Coordinadas - Macroseccion</t>
+          <t>ICS2523_1_2_Sec_Coordinadas - Macroseccion</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>ICS3413_2_3_Sec_Coordinadas - Macroseccion</t>
+          <t>ICS2613_Coordinado - Macroseccion</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>IIC1103_Coordinado - Macroseccion</t>
+          <t>ICS3213_Coordinado - Macroseccion</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>IIC1253_Coordinado - Macroseccion</t>
+          <t>ICS3313_2_3_Sec_Coordinadas - Macroseccion</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>IIC2343_Coordinado - Macroseccion</t>
+          <t>ICS3413_2_3_Sec_Coordinadas - Macroseccion</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>IIC3745_Coordinado - Macroseccion</t>
+          <t>IIC1103_Coordinado - Macroseccion</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>IIQ1003_Coordinado - Macroseccion</t>
+          <t>IIC1253_Coordinado - Macroseccion</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>J7_MS1 - Macroseccion 1</t>
+          <t>IIC2343_Coordinado - Macroseccion</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>MAT1203_Coordinado - Macroseccion</t>
+          <t>IIC3745_Coordinado - Macroseccion</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>MAT1610_Coordinado - Macroseccion</t>
+          <t>IIQ1003_Coordinado - Macroseccion</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>MAT1620_Coordinado - Macroseccion</t>
+          <t>J7_MS1 - Macroseccion 1</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>MAT1630_Coordinado - Macroseccion</t>
+          <t>MAT1203_Coordinado - Macroseccion</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>MAT1640_Coordinado - Macroseccion</t>
+          <t>MAT1610_Coordinado - Macroseccion</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>R2_MS1 - Macroseccion 1</t>
+          <t>MAT1620_Coordinado - Macroseccion</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>R3_MS1 - Macroseccion 1</t>
+          <t>MAT1630_Coordinado - Macroseccion</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>W0_MS1 - Macroseccion 1</t>
+          <t>MAT1640_Coordinado - Macroseccion</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
+        <is>
+          <t>QIM100E_Coordinado - Macroseccion</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>R2_MS1 - Macroseccion 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>R3_MS1 - Macroseccion 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>W0_MS1 - Macroseccion 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
         <is>
           <t>Z8_MS1 - Macroseccion 1</t>
         </is>

</xml_diff>

<commit_message>
Agregado comentarios en prerrequisitos.py, main.py
</commit_message>
<xml_diff>
--- a/Interrogaciones/src/instancia_datos/listado_cursos.xlsx
+++ b/Interrogaciones/src/instancia_datos/listado_cursos.xlsx
@@ -443,357 +443,357 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>IMM2043-1</t>
+          <t>ICM2203-1</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ICC2204-1</t>
+          <t>IEE2343-1</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ICH2204-1</t>
+          <t>ICC3253-1</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>IMM3323-1</t>
+          <t>IMM2213-1</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ICH3374-1</t>
+          <t>ICS2123-3</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ICM2213-1</t>
+          <t>ICT3523-1</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>ICE2633-1</t>
+          <t>IIC3113-2</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>ICM2333-1</t>
+          <t>ICE2114-1</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>ICE2703-1</t>
+          <t>ICT2303-1</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>IMM2013-1</t>
+          <t>IIC3113-1</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ICS3151-1</t>
+          <t>ICE2006-1</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ICS3313-1</t>
+          <t>ICM2313-1</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ICT3283-1</t>
+          <t>IEE2513-1</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ICS3723-1</t>
+          <t>IIC2613-1</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>ICE3443-1</t>
+          <t>IIC2764-1</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ICH2304-1</t>
+          <t>ICH3350-1</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>ICE2020-1</t>
+          <t>IEE2413-1</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>IEE2113-1</t>
+          <t>IEE2103-1</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>IIQ2303-1</t>
+          <t>IEE2613-1</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>ICM3235-1</t>
+          <t>IMM2033-1</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>ICS2123-1</t>
+          <t>ICE2313-1</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>IMM3313-1</t>
+          <t>ICH2124-1</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>ICH2304-2</t>
+          <t>ICH3222-1</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>ICH1005-1</t>
+          <t>ICE2604-1</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>IEE2713-1</t>
+          <t>IMM1003-1</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>IIC2713-2</t>
+          <t>ICC3124-1</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>IIC2713-1</t>
+          <t>IIC1001-1</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>ICS2123-2</t>
+          <t>ICM1001-1</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>ICH3600-1</t>
+          <t>IIQ2003-1</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>IIC2713-3</t>
+          <t>ICM2223-1</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>ICM3243-1</t>
+          <t>ICE3233-1</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>ICE2623-1</t>
+          <t>ICS2523-4</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>ICT3464-1</t>
+          <t>IMM2013-1</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>ICS2023-1</t>
+          <t>ICE2028-1</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>ICC2304-1</t>
+          <t>ICS3582-1</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>IEE3234-1</t>
+          <t>ICM3762-1</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>IEE2463-1</t>
+          <t>IIC2213-1</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>IIC2733-1</t>
+          <t>ICT3623-1</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>IMT3150-1</t>
+          <t>IEE3732-1</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>ICS3413-1</t>
+          <t>IMT3800-1</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>IIQ3343-1</t>
+          <t>ICS2121-1</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>IEE2123-1</t>
+          <t>IMM2003-1</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>ICC3543-1</t>
+          <t>ICM2803-1</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>ICH3364-1</t>
+          <t>IIC2733-1</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>IIC2733-2</t>
+          <t>IMT3150-1</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>ICM2803-1</t>
+          <t>IEE2463-1</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>ICH2214-1</t>
+          <t>ICS2563-1</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>ICE3613-1</t>
+          <t>IEE2213-1</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>ICE2604-1</t>
+          <t>IIQ3343-1</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>IEE2213-1</t>
+          <t>IEE2123-1</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>ICS2563-1</t>
+          <t>ICH2214-1</t>
         </is>
       </c>
     </row>
@@ -821,602 +821,602 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>ICH2574-1</t>
+          <t>IIC2733-2</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>ICH3532-1</t>
+          <t>ICC3543-1</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>ICC3434-1</t>
+          <t>ICE3613-1</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>ICE2028-1</t>
+          <t>ICH3364-1</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>IMM2003-1</t>
+          <t>ICS3413-1</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>ICE3653-1</t>
+          <t>IEE3234-1</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>ICS3811-1</t>
+          <t>ICC2304-1</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>IMM2033-1</t>
+          <t>IMM3323-1</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>IIC3103-1</t>
+          <t>ICS2023-1</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>ICH3350-1</t>
+          <t>ICH3600-1</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>IIC2764-1</t>
+          <t>ICH1005-1</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>ICE2313-1</t>
+          <t>ICT3464-1</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>IEE2103-1</t>
+          <t>IIC2713-1</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>IEE2613-1</t>
+          <t>IIC2713-2</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>IEE2413-1</t>
+          <t>IEE2713-1</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>ICH2124-1</t>
+          <t>ICH2304-2</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>IIQ3643-1</t>
+          <t>ICE2623-1</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>ICE2006-1</t>
+          <t>IIC2713-3</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>IMT2111-1</t>
+          <t>ICM3243-1</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>ICC3264-1</t>
+          <t>ICS2123-2</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>IEE3373-1</t>
+          <t>ICS3811-1</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>ICM3251-1</t>
+          <t>ICE2633-1</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>ICS3762-1</t>
+          <t>IMM3800-1</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>ICE2114-1</t>
+          <t>ICH3532-1</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>ICS2123-3</t>
+          <t>ICE3653-1</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>IMM2213-1</t>
+          <t>ICE2020-1</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>IIC3113-2</t>
+          <t>IMM3313-1</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>IEE2513-1</t>
+          <t>ICH2574-1</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>ICM2313-1</t>
+          <t>IIC3757-1</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>ICC3253-1</t>
+          <t>IMM2043-1</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>IEE2343-1</t>
+          <t>ICH2114-1</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>ICM2203-1</t>
+          <t>IIC3800-1</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>ICT2303-1</t>
+          <t>ICE3413-1</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>ICT3523-1</t>
+          <t>ICS2563-2</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>IIC2613-1</t>
+          <t>ICT3435-1</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>IIC3113-1</t>
+          <t>IMT3130-1</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>IIC3743-1</t>
+          <t>ICM2003-1</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>IMM2053-1</t>
+          <t>ICM2028-1</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>ICE2533-1</t>
+          <t>ICM2413-1</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>ICE3753-1</t>
+          <t>IIC2143-2</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>ICS2523-3</t>
+          <t>IIQ2663-1</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>IMM1003-1</t>
+          <t>ICT2233-1</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>ICM2223-1</t>
+          <t>IIC2143-1</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>ICS2523-4</t>
+          <t>IIC3103-1</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>ICM1001-1</t>
+          <t>ICS3762-1</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>IIC1001-1</t>
+          <t>ICC3264-1</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>IIQ2003-1</t>
+          <t>IMT2111-1</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>ICC3124-1</t>
+          <t>IIQ3643-1</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>ICE3233-1</t>
+          <t>ICM3251-1</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>ICH3222-1</t>
+          <t>IEE3373-1</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>IEE3732-1</t>
+          <t>IIC3743-1</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>IMT3800-1</t>
+          <t>ICE2703-1</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>ICM3762-1</t>
+          <t>ICE2533-1</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>ICS2121-1</t>
+          <t>ICE3753-1</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>IIC2213-1</t>
+          <t>ICS2523-3</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>ICS3582-1</t>
+          <t>IMM2053-1</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>ICT3623-1</t>
+          <t>ICS3151-1</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>IIC3800-1</t>
+          <t>ICS3313-1</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>IIC3757-1</t>
+          <t>ICH2304-1</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>IMM3800-1</t>
+          <t>ICH2204-1</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>IIQ2043-1</t>
+          <t>ICM2333-1</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>IIC2133-1</t>
+          <t>ICE3443-1</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>IIC3242-1</t>
+          <t>ICH3374-1</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>IIC2133-2</t>
+          <t>ICT3283-1</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>ICE3513-1</t>
+          <t>ICS2123-1</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>ICH2114-1</t>
+          <t>IIQ2303-1</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>ICE3663-1</t>
+          <t>IEE2113-1</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>ICM2403-1</t>
+          <t>ICC2204-1</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>ICC1001-1</t>
+          <t>ICS3723-1</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>ICT3435-1</t>
+          <t>ICM3235-1</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>IIC2143-1</t>
+          <t>ICM2213-1</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>IMT3130-1</t>
+          <t>ICC3434-1</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>ICT2233-1</t>
+          <t>ICC3214-1</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>ICM2003-1</t>
+          <t>IIQ2133-1</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>ICM2413-1</t>
+          <t>IIC2333-1</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>IIC2143-2</t>
+          <t>IIC3143-1</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>IIQ2663-1</t>
+          <t>ICC2514-1</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>ICM2028-1</t>
+          <t>ICM2022-1</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>ICS2563-2</t>
+          <t>IIQ2043-1</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>ICE3413-1</t>
+          <t>ICE3513-1</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>IIC2333-1</t>
+          <t>IIC3242-1</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>ICC3214-1</t>
+          <t>ICE3663-1</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>ICC2514-1</t>
+          <t>IIC2133-1</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>IIQ2133-1</t>
+          <t>ICC1001-1</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>IIC3143-1</t>
+          <t>IIC2133-2</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>ICM2022-1</t>
+          <t>ICM2403-1</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Intento (incompleto) de agregar equivalencias a prerrequisitos
</commit_message>
<xml_diff>
--- a/Interrogaciones/src/instancia_datos/listado_cursos.xlsx
+++ b/Interrogaciones/src/instancia_datos/listado_cursos.xlsx
@@ -443,252 +443,252 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ICM2203-1</t>
+          <t>ICC2304-1</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>IEE2343-1</t>
+          <t>IIC2713-1</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ICC3253-1</t>
+          <t>ICM3243-1</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>IMM2213-1</t>
+          <t>ICH3600-1</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ICS2123-3</t>
+          <t>ICH1005-1</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ICT3523-1</t>
+          <t>ICH2304-2</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>IIC3113-2</t>
+          <t>ICS2023-1</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>ICE2114-1</t>
+          <t>IIC2713-3</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>ICT2303-1</t>
+          <t>ICE2623-1</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>IIC3113-1</t>
+          <t>ICS2123-2</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ICE2006-1</t>
+          <t>IMM3323-1</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ICM2313-1</t>
+          <t>IIC2713-2</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>IEE2513-1</t>
+          <t>ICS3811-1</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>IIC2613-1</t>
+          <t>ICT3464-1</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>IIC2764-1</t>
+          <t>IEE2713-1</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ICH3350-1</t>
+          <t>ICM3762-1</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>IEE2413-1</t>
+          <t>ICS2121-1</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>IEE2103-1</t>
+          <t>IIC3800-1</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>IEE2613-1</t>
+          <t>ICS3582-1</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>IMM2033-1</t>
+          <t>IMM2003-1</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>ICE2313-1</t>
+          <t>ICE2028-1</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>ICH2124-1</t>
+          <t>IMT3800-1</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>ICH3222-1</t>
+          <t>IMM3800-1</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>ICE2604-1</t>
+          <t>IIC3743-1</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>IMM1003-1</t>
+          <t>ICS3413-1</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>ICC3124-1</t>
+          <t>ICH2214-1</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>IIC1001-1</t>
+          <t>IIC2733-1</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>ICM1001-1</t>
+          <t>ICH3350-1</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>IIQ2003-1</t>
+          <t>ICE3653-1</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>ICM2223-1</t>
+          <t>IMM2033-1</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>ICE3233-1</t>
+          <t>ICE3124-1</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>ICS2523-4</t>
+          <t>IIC2764-1</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>IMM2013-1</t>
+          <t>IEE2213-1</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>ICE2028-1</t>
+          <t>IIC2733-2</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>ICS3582-1</t>
+          <t>IEE2123-1</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>ICM3762-1</t>
+          <t>IEE3732-1</t>
         </is>
       </c>
     </row>
@@ -709,714 +709,714 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>IEE3732-1</t>
+          <t>ICS2523-4</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>IMT3800-1</t>
+          <t>ICH3222-1</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>ICS2121-1</t>
+          <t>ICE2633-1</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>IMM2003-1</t>
+          <t>IIC3757-1</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>ICM2803-1</t>
+          <t>IMT2111-1</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>IIC2733-1</t>
+          <t>ICE2703-1</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>IMT3150-1</t>
+          <t>ICS3762-1</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>IEE2463-1</t>
+          <t>IEE3373-1</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>ICS2563-1</t>
+          <t>ICM3251-1</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>IEE2213-1</t>
+          <t>IIQ3643-1</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>IIQ3343-1</t>
+          <t>ICC3264-1</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>IEE2123-1</t>
+          <t>ICM2403-1</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>ICH2214-1</t>
+          <t>IIQ2043-1</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>ICE3124-1</t>
+          <t>ICE3663-1</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>IIQ2673-1</t>
+          <t>ICH2114-1</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>ICC2105-1</t>
+          <t>IIC2133-1</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>IIC2733-2</t>
+          <t>ICC1001-1</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>ICC3543-1</t>
+          <t>ICE3513-1</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>ICE3613-1</t>
+          <t>IIC3242-1</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>ICH3364-1</t>
+          <t>ICC3434-1</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>ICS3413-1</t>
+          <t>IIC2133-2</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>IEE3234-1</t>
+          <t>IEE2113-1</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>ICC2304-1</t>
+          <t>IMM2043-1</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>IMM3323-1</t>
+          <t>IMM2013-1</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>ICS2023-1</t>
+          <t>ICH2204-1</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>ICH3600-1</t>
+          <t>ICS2123-1</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>ICH1005-1</t>
+          <t>ICH2304-1</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>ICT3464-1</t>
+          <t>ICH3374-1</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>IIC2713-1</t>
+          <t>ICC2204-1</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>IIC2713-2</t>
+          <t>ICM2333-1</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>IEE2713-1</t>
+          <t>ICT3283-1</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>ICH2304-2</t>
+          <t>ICM2213-1</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>ICE2623-1</t>
+          <t>ICS3723-1</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>IIC2713-3</t>
+          <t>ICM3235-1</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>ICM3243-1</t>
+          <t>ICS3313-1</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>ICS2123-2</t>
+          <t>ICE3443-1</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>ICS3811-1</t>
+          <t>IIQ2303-1</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>ICE2633-1</t>
+          <t>ICS3151-1</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>IMM3800-1</t>
+          <t>ICE2020-1</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>ICH3532-1</t>
+          <t>IMM3313-1</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>ICE3653-1</t>
+          <t>IEE2463-1</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>ICE2020-1</t>
+          <t>ICE2604-1</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>IMM3313-1</t>
+          <t>ICC3543-1</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>ICH2574-1</t>
+          <t>ICC2105-1</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>IIC3757-1</t>
+          <t>ICE3613-1</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>IMM2043-1</t>
+          <t>IIQ3343-1</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>ICH2114-1</t>
+          <t>IIQ2673-1</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>IIC3800-1</t>
+          <t>ICH3364-1</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>ICE3413-1</t>
+          <t>IMT3150-1</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>ICS2563-2</t>
+          <t>ICS2563-1</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>ICT3435-1</t>
+          <t>ICM2803-1</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>IMT3130-1</t>
+          <t>IEE3234-1</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>ICM2003-1</t>
+          <t>ICH2574-1</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>ICM2028-1</t>
+          <t>ICH3532-1</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>ICM2413-1</t>
+          <t>ICE3233-1</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>IIC2143-2</t>
+          <t>ICM2223-1</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>IIQ2663-1</t>
+          <t>IIQ2003-1</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>ICT2233-1</t>
+          <t>ICC3124-1</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>IIC2143-1</t>
+          <t>IMM1003-1</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>IIC3103-1</t>
+          <t>ICM1001-1</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>ICS3762-1</t>
+          <t>IIC1001-1</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>ICC3264-1</t>
+          <t>IMT3130-1</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>IMT2111-1</t>
+          <t>ICM2003-1</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>IIQ3643-1</t>
+          <t>ICH2124-1</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>ICM3251-1</t>
+          <t>IEE2613-1</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>IEE3373-1</t>
+          <t>ICT2233-1</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>IIC3743-1</t>
+          <t>ICT3435-1</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>ICE2703-1</t>
+          <t>ICM2413-1</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>ICE2533-1</t>
+          <t>ICS2563-2</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>ICE3753-1</t>
+          <t>ICM2028-1</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>ICS2523-3</t>
+          <t>IEE2103-1</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>IMM2053-1</t>
+          <t>IIC2143-2</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>ICS3151-1</t>
+          <t>ICE3413-1</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>ICS3313-1</t>
+          <t>IIC2143-1</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>ICH2304-1</t>
+          <t>IEE2413-1</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>ICH2204-1</t>
+          <t>IIQ2663-1</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>ICM2333-1</t>
+          <t>ICE2313-1</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>ICE3443-1</t>
+          <t>IIC3103-1</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>ICH3374-1</t>
+          <t>ICS2523-3</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>ICT3283-1</t>
+          <t>ICE3753-1</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>ICS2123-1</t>
+          <t>IMM2053-1</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>IIQ2303-1</t>
+          <t>ICE2533-1</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>IEE2113-1</t>
+          <t>ICE2114-1</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>ICC2204-1</t>
+          <t>ICE2006-1</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>ICS3723-1</t>
+          <t>ICT2303-1</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>ICM3235-1</t>
+          <t>IIC3113-2</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>ICM2213-1</t>
+          <t>IIC2613-1</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>ICC3434-1</t>
+          <t>IIC3113-1</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>ICC3214-1</t>
+          <t>ICT3523-1</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>IIQ2133-1</t>
+          <t>ICS2123-3</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>IIC2333-1</t>
+          <t>ICM2203-1</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>IIC3143-1</t>
+          <t>ICC3253-1</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>ICC2514-1</t>
+          <t>IMM2213-1</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>ICM2022-1</t>
+          <t>ICM2313-1</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>IIQ2043-1</t>
+          <t>IEE2343-1</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>ICE3513-1</t>
+          <t>IEE2513-1</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>IIC3242-1</t>
+          <t>ICM2022-1</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>ICE3663-1</t>
+          <t>IIQ2133-1</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>IIC2133-1</t>
+          <t>ICC2514-1</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>ICC1001-1</t>
+          <t>ICC3214-1</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>IIC2133-2</t>
+          <t>IIC3143-1</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>ICM2403-1</t>
+          <t>IIC2333-1</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Agregados cursos mat, fis, qim a prerrequisitos
Ojo que tiene un error, porque no se están considerando varios cursos fmat en el modelo.

Del main, se editaron las funciones:
cusos_con_pruebas (creé nuevas para incluir mat y fisqim)
cursos_mod_dipre (saqué parámetros hardcodeados, ya estaba de antes el cambio de incluir cursos fis y qim)
reemplazar_siglas_con_macrosecciones (metí el logging debug adentro del if len(lista...) != 0 para que dejara de tirar un error)
</commit_message>
<xml_diff>
--- a/Interrogaciones/src/instancia_datos/listado_cursos.xlsx
+++ b/Interrogaciones/src/instancia_datos/listado_cursos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A177"/>
+  <dimension ref="A1:A167"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,980 +443,980 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ICC2304-1</t>
+          <t>IIC3757-1</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>IIC2713-1</t>
+          <t>ICH2304-2</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ICM3243-1</t>
+          <t>ICE2623-1</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ICH3600-1</t>
+          <t>IEE3373-1</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ICH1005-1</t>
+          <t>IIC3743-1</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ICH2304-2</t>
+          <t>ICM3251-1</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>ICS2023-1</t>
+          <t>IMT2111-1</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>IIC2713-3</t>
+          <t>ICE2703-1</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>ICE2623-1</t>
+          <t>IIC3800-1</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ICS2123-2</t>
+          <t>ICC3264-1</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>IMM3323-1</t>
+          <t>ICS3762-1</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>IIC2713-2</t>
+          <t>IIQ3643-1</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ICS3811-1</t>
+          <t>ICE3513-1</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ICT3464-1</t>
+          <t>IIC2133-1</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>IEE2713-1</t>
+          <t>ICM2403-1</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ICM3762-1</t>
+          <t>IIC2133-2</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>ICS2121-1</t>
+          <t>ICC1001-1</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>IIC3800-1</t>
+          <t>IIC3242-1</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>ICS3582-1</t>
+          <t>ICC3434-1</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>IMM2003-1</t>
+          <t>ICH2114-1</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>ICE2028-1</t>
+          <t>ICE3663-1</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>IMT3800-1</t>
+          <t>IIQ2043-1</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>IMM3800-1</t>
+          <t>IMM2003-1</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>IIC3743-1</t>
+          <t>ICE2028-1</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>ICS3413-1</t>
+          <t>IMM2043-1</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>ICH2214-1</t>
+          <t>IMM3313-1</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>IIC2733-1</t>
+          <t>ICM3243-1</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>ICH3350-1</t>
+          <t>IMM3323-1</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>ICE3653-1</t>
+          <t>ICH3600-1</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>IMM2033-1</t>
+          <t>IEE2713-1</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>ICE3124-1</t>
+          <t>IIC2713-2</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>IIC2764-1</t>
+          <t>ICC2304-1</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>IEE2213-1</t>
+          <t>ICT3464-1</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>IIC2733-2</t>
+          <t>IIC2713-3</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>IEE2123-1</t>
+          <t>ICH1005-1</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>IEE3732-1</t>
+          <t>ICS2123-2</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>IIC2213-1</t>
+          <t>ICS2023-1</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>ICT3623-1</t>
+          <t>IIC2713-1</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>ICS2523-4</t>
+          <t>ICS3811-1</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>ICH3222-1</t>
+          <t>IIC3103-1</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>ICE2633-1</t>
+          <t>ICE2006-1</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>IIC3757-1</t>
+          <t>ICE2114-1</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>IMT2111-1</t>
+          <t>ICM2333-1</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>ICE2703-1</t>
+          <t>IEE2113-1</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>ICS3762-1</t>
+          <t>ICH3374-1</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>IEE3373-1</t>
+          <t>ICS3723-1</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>ICM3251-1</t>
+          <t>ICH2304-1</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>IIQ3643-1</t>
+          <t>IMM2013-1</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>ICC3264-1</t>
+          <t>ICH2204-1</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>ICM2403-1</t>
+          <t>ICM3235-1</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>IIQ2043-1</t>
+          <t>ICE2633-1</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>ICE3663-1</t>
+          <t>IIQ2303-1</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>ICH2114-1</t>
+          <t>ICE3443-1</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>IIC2133-1</t>
+          <t>ICS3313-1</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>ICC1001-1</t>
+          <t>ICE2020-1</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>ICE3513-1</t>
+          <t>ICC2204-1</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>IIC3242-1</t>
+          <t>ICS2123-1</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>ICC3434-1</t>
+          <t>ICT3283-1</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>IIC2133-2</t>
+          <t>ICM2213-1</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>IEE2113-1</t>
+          <t>ICS3151-1</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>IMM2043-1</t>
+          <t>ICM3762-1</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>IMM2013-1</t>
+          <t>IMT3800-1</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>ICH2204-1</t>
+          <t>ICS2121-1</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>ICS2123-1</t>
+          <t>ICS3582-1</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>ICH2304-1</t>
+          <t>IIC3113-2</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>ICH3374-1</t>
+          <t>ICM2313-1</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>ICC2204-1</t>
+          <t>ICS2123-3</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>ICM2333-1</t>
+          <t>ICC3253-1</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>ICT3283-1</t>
+          <t>IIC2613-1</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>ICM2213-1</t>
+          <t>IEE2513-1</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>ICS3723-1</t>
+          <t>IMM2213-1</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>ICM3235-1</t>
+          <t>ICM2203-1</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>ICS3313-1</t>
+          <t>IIC3113-1</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>ICE3443-1</t>
+          <t>IEE2343-1</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>IIQ2303-1</t>
+          <t>ICT3523-1</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>ICS3151-1</t>
+          <t>ICT2303-1</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>ICE2020-1</t>
+          <t>IIC2764-1</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>IMM3313-1</t>
+          <t>ICH3532-1</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>IEE2463-1</t>
+          <t>ICH2574-1</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>ICE2604-1</t>
+          <t>ICE3653-1</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>ICC3543-1</t>
+          <t>IMM2033-1</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>ICC2105-1</t>
+          <t>IEE2613-1</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>ICE3613-1</t>
+          <t>ICH2124-1</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>IIQ3343-1</t>
+          <t>ICE2313-1</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>IIQ2673-1</t>
+          <t>IEE2103-1</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>ICH3364-1</t>
+          <t>IEE2413-1</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>IMT3150-1</t>
+          <t>ICH3350-1</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>ICS2563-1</t>
+          <t>ICE2533-1</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>ICM2803-1</t>
+          <t>IEE2463-1</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>IEE3234-1</t>
+          <t>IMM2053-1</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>ICH2574-1</t>
+          <t>ICE3753-1</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>ICH3532-1</t>
+          <t>ICS2523-3</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>ICE3233-1</t>
+          <t>ICS3413-1</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>ICM2223-1</t>
+          <t>IEE2213-1</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>IIQ2003-1</t>
+          <t>ICH2214-1</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>ICC3124-1</t>
+          <t>IEE2123-1</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>IMM1003-1</t>
+          <t>ICE3124-1</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>ICM1001-1</t>
+          <t>IIC2733-1</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>IIC1001-1</t>
+          <t>IIC2733-2</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>IMT3130-1</t>
+          <t>ICH3222-1</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>ICM2003-1</t>
+          <t>IEE3732-1</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>ICH2124-1</t>
+          <t>ICT3623-1</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>IEE2613-1</t>
+          <t>IIC2213-1</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>ICT2233-1</t>
+          <t>ICS2523-4</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>ICT3435-1</t>
+          <t>IMM3800-1</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>ICM2413-1</t>
+          <t>ICC3543-1</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>ICS2563-2</t>
+          <t>ICC2105-1</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>ICM2028-1</t>
+          <t>ICE3613-1</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>IEE2103-1</t>
+          <t>ICH3364-1</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>IIC2143-2</t>
+          <t>IEE3234-1</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>ICE3413-1</t>
+          <t>IMT3150-1</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>IIC2143-1</t>
+          <t>ICE2604-1</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>IEE2413-1</t>
+          <t>ICM2803-1</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>IIQ2663-1</t>
+          <t>IIQ3343-1</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>ICE2313-1</t>
+          <t>ICS2563-1</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>IIC3103-1</t>
+          <t>IIQ2673-1</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>ICS2523-3</t>
+          <t>ICM1001-1</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>ICE3753-1</t>
+          <t>ICM2223-1</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>IMM2053-1</t>
+          <t>IIC1001-1</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>ICE2533-1</t>
+          <t>IMM1003-1</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>ICE2114-1</t>
+          <t>IIQ2003-1</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>ICE2006-1</t>
+          <t>ICE3233-1</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>ICT2303-1</t>
+          <t>ICC3124-1</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>IIC3113-2</t>
+          <t>ICS2563-2</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>IIC2613-1</t>
+          <t>IIC2143-1</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>IIC3113-1</t>
+          <t>ICE3413-1</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>ICT3523-1</t>
+          <t>IMT3130-1</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>ICS2123-3</t>
+          <t>ICT2233-1</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>ICM2203-1</t>
+          <t>ICT3435-1</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>ICC3253-1</t>
+          <t>ICM2003-1</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>IMM2213-1</t>
+          <t>ICM2028-1</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>ICM2313-1</t>
+          <t>IIQ2663-1</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>IEE2343-1</t>
+          <t>ICM2413-1</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>IEE2513-1</t>
+          <t>IIC2143-2</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>ICM2022-1</t>
+          <t>ICC2514-1</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>IIQ2133-1</t>
+          <t>IIC3143-1</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>ICC2514-1</t>
+          <t>IIC2333-1</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>ICC3214-1</t>
+          <t>ICM2022-1</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>IIC3143-1</t>
+          <t>ICC3214-1</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>IIC2333-1</t>
+          <t>IIQ2133-1</t>
         </is>
       </c>
     </row>
@@ -1451,222 +1451,152 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>EYP1113_Coordinado - Macroseccion</t>
+          <t>I5_MS1 - Macroseccion 1</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>FIS1514_Coordinado - Macroseccion</t>
+          <t>I6_MS1 - Macroseccion 1</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>FIS1523_Coordinado - Macroseccion</t>
+          <t>ICE1514_Coordinado - Macroseccion</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>FIS1533_Coordinado - Macroseccion</t>
+          <t>ICH1104_Coordinado - Macroseccion</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>I5_MS1 - Macroseccion 1</t>
+          <t>ICM2503_Coordinado - Macroseccion</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>I6_MS1 - Macroseccion 1</t>
+          <t>ICS1113_Coordinado - Macroseccion</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>ICE1514_Coordinado - Macroseccion</t>
+          <t>ICS1513_Coordinado - Macroseccion</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>ICH1104_Coordinado - Macroseccion</t>
+          <t>ICS2523_1_2_Sec_Coordinadas - Macroseccion</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>ICM2503_Coordinado - Macroseccion</t>
+          <t>ICS2613_Coordinado - Macroseccion</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>ICS1113_Coordinado - Macroseccion</t>
+          <t>ICS3213_Coordinado - Macroseccion</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>ICS1513_Coordinado - Macroseccion</t>
+          <t>ICS3313_2_3_Sec_Coordinadas - Macroseccion</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>ICS2523_1_2_Sec_Coordinadas - Macroseccion</t>
+          <t>ICS3413_2_3_Sec_Coordinadas - Macroseccion</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>ICS2613_Coordinado - Macroseccion</t>
+          <t>IIC1103_Coordinado - Macroseccion</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>ICS3213_Coordinado - Macroseccion</t>
+          <t>IIC1253_Coordinado - Macroseccion</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>ICS3313_2_3_Sec_Coordinadas - Macroseccion</t>
+          <t>IIC2343_Coordinado - Macroseccion</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>ICS3413_2_3_Sec_Coordinadas - Macroseccion</t>
+          <t>IIC3745_Coordinado - Macroseccion</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>IIC1103_Coordinado - Macroseccion</t>
+          <t>IIQ1003_Coordinado - Macroseccion</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>IIC1253_Coordinado - Macroseccion</t>
+          <t>J7_MS1 - Macroseccion 1</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>IIC2343_Coordinado - Macroseccion</t>
+          <t>R2_MS1 - Macroseccion 1</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>IIC3745_Coordinado - Macroseccion</t>
+          <t>R3_MS1 - Macroseccion 1</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>IIQ1003_Coordinado - Macroseccion</t>
+          <t>W0_MS1 - Macroseccion 1</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
-        <is>
-          <t>J7_MS1 - Macroseccion 1</t>
-        </is>
-      </c>
-    </row>
-    <row r="168">
-      <c r="A168" t="inlineStr">
-        <is>
-          <t>MAT1203_Coordinado - Macroseccion</t>
-        </is>
-      </c>
-    </row>
-    <row r="169">
-      <c r="A169" t="inlineStr">
-        <is>
-          <t>MAT1610_Coordinado - Macroseccion</t>
-        </is>
-      </c>
-    </row>
-    <row r="170">
-      <c r="A170" t="inlineStr">
-        <is>
-          <t>MAT1620_Coordinado - Macroseccion</t>
-        </is>
-      </c>
-    </row>
-    <row r="171">
-      <c r="A171" t="inlineStr">
-        <is>
-          <t>MAT1630_Coordinado - Macroseccion</t>
-        </is>
-      </c>
-    </row>
-    <row r="172">
-      <c r="A172" t="inlineStr">
-        <is>
-          <t>MAT1640_Coordinado - Macroseccion</t>
-        </is>
-      </c>
-    </row>
-    <row r="173">
-      <c r="A173" t="inlineStr">
-        <is>
-          <t>QIM100E_Coordinado - Macroseccion</t>
-        </is>
-      </c>
-    </row>
-    <row r="174">
-      <c r="A174" t="inlineStr">
-        <is>
-          <t>R2_MS1 - Macroseccion 1</t>
-        </is>
-      </c>
-    </row>
-    <row r="175">
-      <c r="A175" t="inlineStr">
-        <is>
-          <t>R3_MS1 - Macroseccion 1</t>
-        </is>
-      </c>
-    </row>
-    <row r="176">
-      <c r="A176" t="inlineStr">
-        <is>
-          <t>W0_MS1 - Macroseccion 1</t>
-        </is>
-      </c>
-    </row>
-    <row r="177">
-      <c r="A177" t="inlineStr">
         <is>
           <t>Z8_MS1 - Macroseccion 1</t>
         </is>

</xml_diff>

<commit_message>
Inclusión a prerrequisitos de cursos FIS, QIM y MAT
1. Tuve que meter los cursos fisqim al dataframe que creaba las macrosecciones (porque antes sólo incluía a los mat)
2. Metí los cursos fis,qim y mat al dataframe de todos los cursos, que es el dataframe "dataframe_ing"
3. Tmb metí los cursos fisqim mat a dataframe con los horarios, pq caché antes que no los pescaba (y al final muchos, como son coordinados, tienen intersección vacía y me empezó a tirar error pero lo arreglé)
4. Después dejaron de aparecer los cursos fis qim y mat en los cursos que entraban al modelo, no me acuerdo por qué era específicamente pero lo solucioné al hacer coincidir los cursos que estaban en ambos dataframes principales
5. Empezaron a aparecer los cursos fisqimmat con 0 vacantes en el modelo, porque al guardar las vacantes generaba un nuevo dataframe en el que, por un cambio que hice, si no se le entregaba el parámetro, no consideraba cursos de fmat, y antes nunca consideraba cursos fis y qim
</commit_message>
<xml_diff>
--- a/Interrogaciones/src/instancia_datos/listado_cursos.xlsx
+++ b/Interrogaciones/src/instancia_datos/listado_cursos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A167"/>
+  <dimension ref="A1:A178"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,980 +443,980 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>IIC3757-1</t>
+          <t>ICS2121-1</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ICH2304-2</t>
+          <t>IMM3800-1</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ICE2623-1</t>
+          <t>IIC2733-1</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>IEE3373-1</t>
+          <t>IEE2213-1</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>IIC3743-1</t>
+          <t>IIQ3343-1</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ICM3251-1</t>
+          <t>IMT3150-1</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>IMT2111-1</t>
+          <t>ICE2604-1</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>ICE2703-1</t>
+          <t>IEE2463-1</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>IIC3800-1</t>
+          <t>ICH3364-1</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ICC3264-1</t>
+          <t>ICM2803-1</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ICS3762-1</t>
+          <t>IIQ2673-1</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>IIQ3643-1</t>
+          <t>ICC2105-1</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ICE3513-1</t>
+          <t>IIC2733-2</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>IIC2133-1</t>
+          <t>ICC3543-1</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>ICM2403-1</t>
+          <t>ICE3613-1</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>IIC2133-2</t>
+          <t>IEE3234-1</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>ICC1001-1</t>
+          <t>ICS2563-1</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>IIC3242-1</t>
+          <t>ICH2214-1</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>ICC3434-1</t>
+          <t>ICE3124-1</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>ICH2114-1</t>
+          <t>IEE2123-1</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>ICE3663-1</t>
+          <t>ICS3413-1</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>IIQ2043-1</t>
+          <t>IMT3800-1</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>IMM2003-1</t>
+          <t>ICE2028-1</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>ICE2028-1</t>
+          <t>ICS3582-1</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>IMM2043-1</t>
+          <t>IIC3800-1</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>IMM3313-1</t>
+          <t>ICM3762-1</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>ICM3243-1</t>
+          <t>IMM2003-1</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>IMM3323-1</t>
+          <t>ICS2123-2</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>ICH3600-1</t>
+          <t>IIC2713-3</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>IEE2713-1</t>
+          <t>ICS2023-1</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>IIC2713-2</t>
+          <t>ICM3243-1</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>ICC2304-1</t>
+          <t>ICT3464-1</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>ICT3464-1</t>
+          <t>ICC2304-1</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>IIC2713-3</t>
+          <t>ICH2304-2</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>ICH1005-1</t>
+          <t>IEE2713-1</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>ICS2123-2</t>
+          <t>IMM3323-1</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>ICS2023-1</t>
+          <t>IIC2713-1</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>IIC2713-1</t>
+          <t>ICH1005-1</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>ICS3811-1</t>
+          <t>ICH3600-1</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>IIC3103-1</t>
+          <t>ICE2623-1</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>ICE2006-1</t>
+          <t>IIC2713-2</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>ICE2114-1</t>
+          <t>ICS3811-1</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>ICM2333-1</t>
+          <t>ICT3623-1</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>IEE2113-1</t>
+          <t>ICS2523-4</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>ICH3374-1</t>
+          <t>IEE3732-1</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>ICS3723-1</t>
+          <t>ICH3222-1</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>ICH2304-1</t>
+          <t>IIC2213-1</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>IMM2013-1</t>
+          <t>ICE2633-1</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>ICH2204-1</t>
+          <t>IMM2033-1</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>ICM3235-1</t>
+          <t>IIC3103-1</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>ICE2633-1</t>
+          <t>IMT2111-1</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>IIQ2303-1</t>
+          <t>ICM3251-1</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>ICE3443-1</t>
+          <t>ICS3762-1</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>ICS3313-1</t>
+          <t>ICE2006-1</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>ICE2020-1</t>
+          <t>ICC3264-1</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>ICC2204-1</t>
+          <t>ICE2114-1</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>ICS2123-1</t>
+          <t>IIQ3643-1</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>ICT3283-1</t>
+          <t>IEE3373-1</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>ICM2213-1</t>
+          <t>IIC3743-1</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>ICS3151-1</t>
+          <t>IIC2613-1</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>ICM3762-1</t>
+          <t>IIC2764-1</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>IMT3800-1</t>
+          <t>ICM2313-1</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>ICS2121-1</t>
+          <t>IMM2213-1</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>ICS3582-1</t>
+          <t>IIC3113-1</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>IIC3113-2</t>
+          <t>ICT2303-1</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>ICM2313-1</t>
+          <t>ICT3523-1</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>ICS2123-3</t>
+          <t>ICC3253-1</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>ICC3253-1</t>
+          <t>ICM2203-1</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>IIC2613-1</t>
+          <t>IEE2343-1</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>IEE2513-1</t>
+          <t>ICS2123-3</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>IMM2213-1</t>
+          <t>IEE2513-1</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>ICM2203-1</t>
+          <t>IIC3113-2</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>IIC3113-1</t>
+          <t>ICE3653-1</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>IEE2343-1</t>
+          <t>ICH3350-1</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>ICT3523-1</t>
+          <t>IEE2103-1</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>ICT2303-1</t>
+          <t>ICE2313-1</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>IIC2764-1</t>
+          <t>ICH2124-1</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>ICH3532-1</t>
+          <t>IEE2613-1</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>ICH2574-1</t>
+          <t>IEE2413-1</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>ICE3653-1</t>
+          <t>IIC2333-1</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>IMM2033-1</t>
+          <t>ICC3214-1</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>IEE2613-1</t>
+          <t>IIC3143-1</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>ICH2124-1</t>
+          <t>IIQ2133-1</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>ICE2313-1</t>
+          <t>ICC2514-1</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>IEE2103-1</t>
+          <t>ICE3753-1</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>IEE2413-1</t>
+          <t>IMM2053-1</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>ICH3350-1</t>
+          <t>ICS2523-3</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>ICE2533-1</t>
+          <t>ICM2022-1</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>IEE2463-1</t>
+          <t>ICE2533-1</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>IMM2053-1</t>
+          <t>IIC3757-1</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>ICE3753-1</t>
+          <t>ICE2703-1</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>ICS2523-3</t>
+          <t>IMM2043-1</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>ICS3413-1</t>
+          <t>ICH2114-1</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>IEE2213-1</t>
+          <t>IMM3313-1</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>ICH2214-1</t>
+          <t>ICE3663-1</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>IEE2123-1</t>
+          <t>ICM2403-1</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>ICE3124-1</t>
+          <t>IIC3242-1</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>IIC2733-1</t>
+          <t>ICC1001-1</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>IIC2733-2</t>
+          <t>IIC2133-1</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>ICH3222-1</t>
+          <t>IIQ2043-1</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>IEE3732-1</t>
+          <t>ICE3513-1</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>ICT3623-1</t>
+          <t>ICC3434-1</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>IIC2213-1</t>
+          <t>IIC2133-2</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>ICS2523-4</t>
+          <t>ICM2213-1</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>IMM3800-1</t>
+          <t>IEE2113-1</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>ICC3543-1</t>
+          <t>ICT3283-1</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>ICC2105-1</t>
+          <t>ICH2204-1</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>ICE3613-1</t>
+          <t>IIQ2303-1</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>ICH3364-1</t>
+          <t>ICM2333-1</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>IEE3234-1</t>
+          <t>ICS3723-1</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>IMT3150-1</t>
+          <t>ICH2304-1</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>ICE2604-1</t>
+          <t>ICC2204-1</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>ICM2803-1</t>
+          <t>ICE2020-1</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>IIQ3343-1</t>
+          <t>ICS3313-1</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>ICS2563-1</t>
+          <t>ICE3443-1</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>IIQ2673-1</t>
+          <t>ICS2123-1</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>ICM1001-1</t>
+          <t>ICH3374-1</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>ICM2223-1</t>
+          <t>ICM3235-1</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>IIC1001-1</t>
+          <t>ICS3151-1</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>IMM1003-1</t>
+          <t>IMM2013-1</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>IIQ2003-1</t>
+          <t>ICH2574-1</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>ICE3233-1</t>
+          <t>ICH3532-1</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>ICC3124-1</t>
+          <t>ICE3233-1</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>ICS2563-2</t>
+          <t>ICM1001-1</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>IIC2143-1</t>
+          <t>ICM2223-1</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>ICE3413-1</t>
+          <t>IIQ2003-1</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>IMT3130-1</t>
+          <t>ICC3124-1</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>ICT2233-1</t>
+          <t>IIC1001-1</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>ICT3435-1</t>
+          <t>IMM1003-1</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>ICM2003-1</t>
+          <t>ICT2233-1</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>ICM2028-1</t>
+          <t>IIC2143-2</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>IIQ2663-1</t>
+          <t>IMT3130-1</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>ICM2413-1</t>
+          <t>IIC2143-1</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>IIC2143-2</t>
+          <t>ICM2413-1</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>ICC2514-1</t>
+          <t>ICE3413-1</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>IIC3143-1</t>
+          <t>ICS2563-2</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>IIC2333-1</t>
+          <t>ICT3435-1</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>ICM2022-1</t>
+          <t>ICM2003-1</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>ICC3214-1</t>
+          <t>ICM2028-1</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>IIQ2133-1</t>
+          <t>IIQ2663-1</t>
         </is>
       </c>
     </row>
@@ -1599,6 +1599,83 @@
       <c r="A167" t="inlineStr">
         <is>
           <t>Z8_MS1 - Macroseccion 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>EYP1113_Coordinado - Macroseccion</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>FIS1514_Coordinado - Macroseccion</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>FIS1523_Coordinado - Macroseccion</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>FIS1533_Coordinado - Macroseccion</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>MAT1203_Coordinado - Macroseccion</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>MAT1207_Coordinado - Macroseccion</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>MAT1610_Coordinado - Macroseccion</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>MAT1620_Coordinado - Macroseccion</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>MAT1630_Coordinado - Macroseccion</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>MAT1640_Coordinado - Macroseccion</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>QIM100E_Coordinado - Macroseccion</t>
         </is>
       </c>
     </row>

</xml_diff>